<commit_message>
Copia de carpeta de estudiante a la carpeta de grupo y envio de correo si no existe expediente
</commit_message>
<xml_diff>
--- a/Registros/Control.xlsx
+++ b/Registros/Control.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +462,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Copiar fecha disponible y agregarla al grupo que necesita; termine el flujo cuando se agrega un nuevo grupo al excel y se crea la carpeta para continuar el flujo
</commit_message>
<xml_diff>
--- a/Registros/Control.xlsx
+++ b/Registros/Control.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13605" windowHeight="7230"/>
   </bookViews>
   <sheets>
     <sheet name="grupos" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Fecha</t>
   </si>
@@ -430,7 +430,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +462,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -476,7 +479,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,6 +504,9 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">

</xml_diff>

<commit_message>
Tratando de obtener datos de la consulta de grupo
</commit_message>
<xml_diff>
--- a/Registros/Control.xlsx
+++ b/Registros/Control.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annel\Yoselin\USAC\IA\Laboratorio\Practica1\IA-Robot\Registros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13605" windowHeight="7230"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13605" windowHeight="7230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="grupos" sheetId="1" r:id="rId1"/>
@@ -20,52 +20,52 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+    <x:ext xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
-    </ext>
+    </x:ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
   <si>
     <t>Fecha</t>
   </si>
   <si>
-    <t>Grupo</t>
-  </si>
-  <si>
     <t>Grupo1</t>
   </si>
   <si>
-    <t>Cantidad</t>
+    <t>3/22/2020</t>
   </si>
   <si>
     <t>Grupo2</t>
   </si>
   <si>
-    <t>3/22/2020</t>
-  </si>
-  <si>
     <t>4/15/2020</t>
   </si>
   <si>
     <t>Uso</t>
   </si>
   <si>
+    <t>x</t>
+  </si>
+  <si>
     <t>6/13/2020</t>
   </si>
   <si>
     <t>8/29/2020</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -109,10 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,44 +430,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -478,49 +477,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44170</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>44170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>